<commit_message>
Projet 'fonctionnel' (à tester avec des IA directement). Manque : Draw et Ecriture en fichier des coups réalisés
</commit_message>
<xml_diff>
--- a/Assets/Resources/Scenarios/Scenarios_Sheets.xlsx
+++ b/Assets/Resources/Scenarios/Scenarios_Sheets.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12330" activeTab="4"/>
+    <workbookView windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Scenario_1" sheetId="1" r:id="rId1"/>
@@ -1115,13 +1115,7 @@
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:F10" totalsRowShown="0">
-  <autoFilter ref="A1:F10">
-    <filterColumn colId="1">
-      <customFilters>
-        <customFilter operator="equal" val="2"/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:F10"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Coup"/>
     <tableColumn id="2" name="Joueur"/>
@@ -1151,13 +1145,7 @@
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau4_6" displayName="Tableau4_6" ref="A1:F11" totalsRowShown="0">
-  <autoFilter ref="A1:F11">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="2"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:F11"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Coup"/>
     <tableColumn id="2" name="Joueur"/>
@@ -1445,8 +1433,8 @@
   <sheetPr/>
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1678,7 +1666,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -1709,7 +1697,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" hidden="1" spans="1:6">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1749,7 +1737,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" hidden="1" spans="1:6">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1789,7 +1777,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" hidden="1" spans="1:6">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1829,7 +1817,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" hidden="1" spans="1:6">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1869,7 +1857,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" hidden="1" spans="1:6">
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1904,7 +1892,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -2063,7 +2051,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -2094,7 +2082,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" hidden="1" spans="1:6">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2134,7 +2122,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" hidden="1" spans="1:6">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2174,7 +2162,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" hidden="1" spans="1:6">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2214,7 +2202,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" hidden="1" spans="1:6">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2254,7 +2242,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" hidden="1" spans="1:6">
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2317,8 +2305,8 @@
   <sheetPr/>
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>

</xml_diff>